<commit_message>
Update all Bank files
</commit_message>
<xml_diff>
--- a/Bank/Bank_Data.xlsx
+++ b/Bank/Bank_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdbb21a5dbde31e1/Documents/UVic/CSC 370/Database Project/Bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{738886CA-2C8A-4F7E-B699-18787AE5989C}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF49B983-9AF2-47B1-A9C4-0D19BBEC21BD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7245" yWindow="525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,10 +397,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated all Bank files
</commit_message>
<xml_diff>
--- a/Bank/Bank_Data.xlsx
+++ b/Bank/Bank_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdbb21a5dbde31e1/Documents/UVic/CSC 370/Database Project/Bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF49B983-9AF2-47B1-A9C4-0D19BBEC21BD}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D19B9B3-1CAA-4DA8-98E3-1C8CE0CA2679}"/>
   <bookViews>
-    <workbookView xWindow="7245" yWindow="525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,7 +360,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +387,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20240519</v>
+        <v>1005151</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>